<commit_message>
Updates to Documentation. Added Espresso Tests for SettingsActivity and TransactionActivity
</commit_message>
<xml_diff>
--- a/Documentation/Final Project Documentation/SD6501_FinalProject_Tests.xlsx
+++ b/Documentation/Final Project Documentation/SD6501_FinalProject_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Dev\BIT\SD6501_Assignment2_Michael_DuToit\Documentation\Final Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61237081-F0A9-446B-BC1F-46CFAC5D98C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487257D0-7862-4A0C-BC0D-7D199599D068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EDED5B4D-BF03-4B30-B7B4-EA90939C677D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="129">
   <si>
     <t>Test ID</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Image</t>
   </si>
   <si>
     <t>AccountUnitTests</t>
@@ -394,7 +391,64 @@
     <t>ES20</t>
   </si>
   <si>
-    <t>AccountBalancesActivity</t>
+    <t>Check that the Floating Action Button is visible, then click on it and check that it takes the user to the Add Transaction View.</t>
+  </si>
+  <si>
+    <t>Check that the Floating Action Button is visible, then click on it and check that it takes the user to the AddAccount view.</t>
+  </si>
+  <si>
+    <t>ES21</t>
+  </si>
+  <si>
+    <t>testAllViewElementsDisplayed</t>
+  </si>
+  <si>
+    <t>Check that the Username and Pin elements are shown to the user.</t>
+  </si>
+  <si>
+    <t>ES22</t>
+  </si>
+  <si>
+    <t>ES23</t>
+  </si>
+  <si>
+    <t>SettingsActivityTest</t>
+  </si>
+  <si>
+    <t>TransactionActivityTest</t>
+  </si>
+  <si>
+    <t>checkViewElementsIncomeDisplayed</t>
+  </si>
+  <si>
+    <t>Check, on the Income Tab, that the view elements are displayed.</t>
+  </si>
+  <si>
+    <t>checkViewElementsExpenseDisplayed</t>
+  </si>
+  <si>
+    <t>Check, on the Expense Tab, that the view elements are displayed.</t>
+  </si>
+  <si>
+    <t>ES24</t>
+  </si>
+  <si>
+    <t>ES25</t>
+  </si>
+  <si>
+    <t>createIncomeTransaction</t>
+  </si>
+  <si>
+    <t>createExpenseTransaction</t>
+  </si>
+  <si>
+    <t>Go to the Income Tab, enter data into all the input fields, then click the Save button. Check that it navigates to the View Transactions Activity.</t>
+  </si>
+  <si>
+    <t>Go to the Expense Tab, enter data into all the input fields, then click the Save button. Check that it navigates to the View Transactions Activity.</t>
+  </si>
+  <si>
+    <t>Figure</t>
   </si>
 </sst>
 </file>
@@ -456,16 +510,16 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -474,19 +528,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -514,35 +568,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E71CAB99-A2F2-4CF9-B0DF-618B930795F7}" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E71CAB99-A2F2-4CF9-B0DF-618B930795F7}" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:H13" xr:uid="{E71CAB99-A2F2-4CF9-B0DF-618B930795F7}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{AAC526E6-E0BB-40DE-BC20-2775B8C148EB}" name="Test ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{6EA3DEB8-279F-40F9-A838-7EC99BC58A40}" name="Test Class" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{AAC526E6-E0BB-40DE-BC20-2775B8C148EB}" name="Test ID" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{6EA3DEB8-279F-40F9-A838-7EC99BC58A40}" name="Test Class" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{5EF4D084-7334-4ACA-8C9A-C22AA2CB7C06}" name="Test Case / Test Method" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{D7383C0E-3DE0-4335-8DB5-6F557268A2FA}" name="Test Description" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{C0D1DB29-7411-40DB-83B0-A5AC03F106A2}" name="Expected Result" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{D7383C0E-3DE0-4335-8DB5-6F557268A2FA}" name="Test Description" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{C0D1DB29-7411-40DB-83B0-A5AC03F106A2}" name="Expected Result" dataDxfId="9"/>
     <tableColumn id="7" xr3:uid="{D1B51E87-80EF-4107-B36B-5470622DE010}" name="Actual Result" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{6CABD4FA-7EB0-4E57-8087-9170AACBCC43}" name="Status" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{EECB0088-7BD1-4F29-8CC6-B05D53198773}" name="Image" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{6CABD4FA-7EB0-4E57-8087-9170AACBCC43}" name="Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{EECB0088-7BD1-4F29-8CC6-B05D53198773}" name="Figure" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44BDAAF5-B155-4F5E-88CC-BF8C8DC7E04C}" name="Table13" displayName="Table13" ref="A1:F19" totalsRowShown="0">
-  <autoFilter ref="A1:F19" xr:uid="{44BDAAF5-B155-4F5E-88CC-BF8C8DC7E04C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{44BDAAF5-B155-4F5E-88CC-BF8C8DC7E04C}" name="Table13" displayName="Table13" ref="A1:F26" totalsRowShown="0">
+  <autoFilter ref="A1:F26" xr:uid="{44BDAAF5-B155-4F5E-88CC-BF8C8DC7E04C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
     <sortCondition ref="B1:B19"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5A28FDFE-56B0-4E69-88C4-64F6B0A6C04C}" name="Test ID" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{EC0ECDBE-58BA-40A5-92BF-FB036279B707}" name="Test Class" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{5A28FDFE-56B0-4E69-88C4-64F6B0A6C04C}" name="Test ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{EC0ECDBE-58BA-40A5-92BF-FB036279B707}" name="Test Class" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{218165FC-B1ED-4716-B233-51AF95A416CC}" name="Test Case / Test Method" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{96585A47-B08E-4291-8849-F7E828491A96}" name="Test Description" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{182A85C6-87BF-48B6-9A92-4DB49708FD20}" name="Status" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{0DF7CB2F-7B0F-4771-A24F-27B7A2AAE3C9}" name="Image" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{182A85C6-87BF-48B6-9A92-4DB49708FD20}" name="Status" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{0DF7CB2F-7B0F-4771-A24F-27B7A2AAE3C9}" name="Figure" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -847,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AFE355-96FE-42FE-9DE0-CD2F1D330447}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,7 +911,8 @@
     <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.5546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="27.6640625" customWidth="1"/>
-    <col min="7" max="8" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -882,320 +937,344 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>7</v>
+      <c r="H1" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H10" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H11" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H12" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="H13" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D15" s="3"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="4:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="4:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1207,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB59A848-E248-4BA0-A1BB-2FC4CAB5537A}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,7 +1299,7 @@
     <col min="3" max="3" width="27.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.88671875" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="6"/>
+    <col min="6" max="6" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1239,276 +1318,508 @@
       <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>7</v>
+      <c r="F1" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>58</v>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>62</v>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>64</v>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>66</v>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>96</v>
+      <c r="E9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>68</v>
+      <c r="E10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="5">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>70</v>
+      <c r="E12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="5">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="5">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="5">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="E17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="5">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the bug where invalid username briefly appeared before logging in with a valid user/pin. Registration sets the logged in user prefs. UAT Testing + Documentation updates.
</commit_message>
<xml_diff>
--- a/Documentation/Final Project Documentation/SD6501_FinalProject_Tests.xlsx
+++ b/Documentation/Final Project Documentation/SD6501_FinalProject_Tests.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Dev\BIT\SD6501_Assignment2_Michael_DuToit\Documentation\Final Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01389EC-99B2-44F4-B6DB-16A4B2CC869F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9C70FB-55DC-4B3B-8E2D-7A4104EB3099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{EDED5B4D-BF03-4B30-B7B4-EA90939C677D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{EDED5B4D-BF03-4B30-B7B4-EA90939C677D}"/>
   </bookViews>
   <sheets>
     <sheet name="UnitTest" sheetId="1" r:id="rId1"/>
     <sheet name="EspressoTests" sheetId="2" r:id="rId2"/>
+    <sheet name="UAT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="144">
   <si>
     <t>Test ID</t>
   </si>
@@ -449,6 +450,51 @@
   </si>
   <si>
     <t>Figure</t>
+  </si>
+  <si>
+    <t>Could you register for a new user account easily?</t>
+  </si>
+  <si>
+    <t>Could you update your user login details?</t>
+  </si>
+  <si>
+    <t>Was all the text readable to you?</t>
+  </si>
+  <si>
+    <t>Could you create an Account?</t>
+  </si>
+  <si>
+    <t>Could you create a Transaction?</t>
+  </si>
+  <si>
+    <t>Was navigating the application intuitive? Did it not take too much thinking on what steps to do to accomplish your goals?</t>
+  </si>
+  <si>
+    <t>Did the application do what you expected?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Yes browsing was intuitive and the application easy to use to accomplish goals like changing user details and performing transactions.</t>
+  </si>
+  <si>
+    <t>Yes, easy to use</t>
+  </si>
+  <si>
+    <t>It was easy and quick.</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>Philip</t>
+  </si>
+  <si>
+    <t>Joseph</t>
   </si>
 </sst>
 </file>
@@ -484,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -504,11 +550,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="24">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -516,22 +595,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -568,17 +647,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E71CAB99-A2F2-4CF9-B0DF-618B930795F7}" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E71CAB99-A2F2-4CF9-B0DF-618B930795F7}" name="Table1" displayName="Table1" ref="A1:H13" totalsRowShown="0" dataDxfId="23">
   <autoFilter ref="A1:H13" xr:uid="{E71CAB99-A2F2-4CF9-B0DF-618B930795F7}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{AAC526E6-E0BB-40DE-BC20-2775B8C148EB}" name="Test ID" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{6EA3DEB8-279F-40F9-A838-7EC99BC58A40}" name="Test Class" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{5EF4D084-7334-4ACA-8C9A-C22AA2CB7C06}" name="Test Case / Test Method" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{D7383C0E-3DE0-4335-8DB5-6F557268A2FA}" name="Test Description" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{C0D1DB29-7411-40DB-83B0-A5AC03F106A2}" name="Expected Result" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{D1B51E87-80EF-4107-B36B-5470622DE010}" name="Actual Result" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{6CABD4FA-7EB0-4E57-8087-9170AACBCC43}" name="Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{EECB0088-7BD1-4F29-8CC6-B05D53198773}" name="Figure" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AAC526E6-E0BB-40DE-BC20-2775B8C148EB}" name="Test ID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{6EA3DEB8-279F-40F9-A838-7EC99BC58A40}" name="Test Class" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{5EF4D084-7334-4ACA-8C9A-C22AA2CB7C06}" name="Test Case / Test Method" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{D7383C0E-3DE0-4335-8DB5-6F557268A2FA}" name="Test Description" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{C0D1DB29-7411-40DB-83B0-A5AC03F106A2}" name="Expected Result" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{D1B51E87-80EF-4107-B36B-5470622DE010}" name="Actual Result" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{6CABD4FA-7EB0-4E57-8087-9170AACBCC43}" name="Status" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{EECB0088-7BD1-4F29-8CC6-B05D53198773}" name="Figure" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -591,12 +670,29 @@
     <sortCondition ref="B1:B19"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5A28FDFE-56B0-4E69-88C4-64F6B0A6C04C}" name="Test ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{EC0ECDBE-58BA-40A5-92BF-FB036279B707}" name="Test Class" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{218165FC-B1ED-4716-B233-51AF95A416CC}" name="Test Case / Test Method" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{96585A47-B08E-4291-8849-F7E828491A96}" name="Test Description" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{182A85C6-87BF-48B6-9A92-4DB49708FD20}" name="Status" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{0DF7CB2F-7B0F-4771-A24F-27B7A2AAE3C9}" name="Figure" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{5A28FDFE-56B0-4E69-88C4-64F6B0A6C04C}" name="Test ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{EC0ECDBE-58BA-40A5-92BF-FB036279B707}" name="Test Class" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{218165FC-B1ED-4716-B233-51AF95A416CC}" name="Test Case / Test Method" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{96585A47-B08E-4291-8849-F7E828491A96}" name="Test Description" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{182A85C6-87BF-48B6-9A92-4DB49708FD20}" name="Status" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{0DF7CB2F-7B0F-4771-A24F-27B7A2AAE3C9}" name="Figure" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0403A5A8-BDBE-4EC0-8478-B97136644E8D}" name="Table3" displayName="Table3" ref="A1:H4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:H4" xr:uid="{0403A5A8-BDBE-4EC0-8478-B97136644E8D}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{3F768492-1C59-47CE-8954-22BDAD29256D}" name="User" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{9F7C5745-BF01-490C-93F3-3A60393DF7A5}" name="Could you register for a new user account easily?" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{093F5141-E42A-4155-9692-BF9F8D23C185}" name="Could you update your user login details?" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{424BD3A3-0F0F-4746-8FD2-1C9965F9AD32}" name="Was all the text readable to you?" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{5C4D5C0E-2134-464E-BBE1-E640094BAA11}" name="Could you create an Account?" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F0CC2469-DA01-47C1-8861-D250C3B5E8B1}" name="Could you create a Transaction?" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{995CF822-795E-47C1-AE1C-B8289D84F060}" name="Was navigating the application intuitive? Did it not take too much thinking on what steps to do to accomplish your goals?"/>
+    <tableColumn id="8" xr3:uid="{A6B29204-A4A3-4EBA-A93F-EE9B54817EF0}" name="Did the application do what you expected?" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1288,7 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB59A848-E248-4BA0-A1BB-2FC4CAB5537A}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1829,4 +1925,136 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B08BB6-67BE-40E0-B747-7349945CACC0}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="42.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="57.109375" customWidth="1"/>
+    <col min="8" max="8" width="37.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>